<commit_message>
Update WMS Deliverables Testing 02Jan2019.xlsx
</commit_message>
<xml_diff>
--- a/WMS Deliverables Testing 02Jan2019.xlsx
+++ b/WMS Deliverables Testing 02Jan2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RDURIASJ\Desktop\VFreight\SIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOQUITAN\OneDrive - Schenker AG\Documents\GitHub\WMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{96A22BCC-EFDD-44FB-B44B-B62DBEA48C73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A4051D48-5BFB-4C46-AB16-14C7615ED5A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{94CC23CC-3793-45CD-B8BE-979C4E7AE973}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8130" xr2:uid="{94CC23CC-3793-45CD-B8BE-979C4E7AE973}"/>
   </bookViews>
   <sheets>
     <sheet name="Listing" sheetId="1" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>ok</t>
   </si>
   <si>
-    <t>Deletion should not allow if there are user associated to the role</t>
-  </si>
-  <si>
     <t>Allocation Strategy</t>
   </si>
   <si>
@@ -322,11 +319,6 @@
     <t>oK</t>
   </si>
   <si>
-    <t>Where to setup the password?
-Contact number should be optional
-If Role is Admin, do we have to select customer or by default all customer?</t>
-  </si>
-  <si>
     <t>ok. Deleted</t>
   </si>
   <si>
@@ -400,13 +392,87 @@
   </si>
   <si>
     <t>email doesn't work yet. To be checked later</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Where to setup the password? - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Auto generated and sent to users ..</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Contact number should be optional - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Done</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If Role is Admin, do we have to select customer or by default all customer? -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> If admin no need to select customer . By default - all customer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Deletion should not allow if there are user associated to the role - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Done</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +484,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -582,6 +663,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -592,18 +685,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -928,49 +1009,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F915EB5C-A5C5-4CCC-B160-03C6AF11F8C8}">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.54296875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="26.81640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="9"/>
-    <col min="5" max="5" width="85.81640625" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="3.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="9"/>
+    <col min="5" max="5" width="85.85546875" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="33"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -983,11 +1064,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="3" t="s">
         <v>54</v>
       </c>
@@ -995,14 +1076,14 @@
         <v>55</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1013,11 +1094,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1025,14 +1106,14 @@
         <v>55</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>5</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1043,11 +1124,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="4" t="s">
         <v>60</v>
       </c>
@@ -1058,11 +1139,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B9" s="31"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="4" t="s">
         <v>62</v>
       </c>
@@ -1073,11 +1154,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>8</v>
       </c>
-      <c r="B10" s="31"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1088,11 +1169,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>9</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1105,11 +1186,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>10</v>
       </c>
-      <c r="B12" s="31"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="4" t="s">
         <v>63</v>
       </c>
@@ -1120,11 +1201,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>11</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="4" t="s">
         <v>64</v>
       </c>
@@ -1135,11 +1216,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>12</v>
       </c>
-      <c r="B14" s="31"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="4" t="s">
         <v>65</v>
       </c>
@@ -1150,11 +1231,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>13</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="4" t="s">
         <v>5</v>
       </c>
@@ -1162,14 +1243,14 @@
         <v>55</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>14</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="4" t="s">
         <v>6</v>
       </c>
@@ -1180,11 +1261,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>15</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1197,11 +1278,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>16</v>
       </c>
-      <c r="B18" s="31"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="4" t="s">
         <v>67</v>
       </c>
@@ -1212,11 +1293,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>17</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
@@ -1227,11 +1308,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>18</v>
       </c>
-      <c r="B20" s="31"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="4" t="s">
         <v>5</v>
       </c>
@@ -1242,23 +1323,23 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B21" s="31"/>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="26"/>
       <c r="C21" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>19</v>
       </c>
-      <c r="B22" s="32"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="4" t="s">
         <v>6</v>
       </c>
@@ -1269,11 +1350,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>20</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="25" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1286,11 +1367,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>21</v>
       </c>
-      <c r="B24" s="31"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="4" t="s">
         <v>70</v>
       </c>
@@ -1298,14 +1379,14 @@
         <v>55</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>22</v>
       </c>
-      <c r="B25" s="31"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="4" t="s">
         <v>4</v>
       </c>
@@ -1316,11 +1397,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>23</v>
       </c>
-      <c r="B26" s="31"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="4" t="s">
         <v>5</v>
       </c>
@@ -1331,11 +1412,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>24</v>
       </c>
-      <c r="B27" s="31"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="4" t="s">
         <v>6</v>
       </c>
@@ -1346,11 +1427,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>25</v>
       </c>
-      <c r="B28" s="32"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="4" t="s">
         <v>12</v>
       </c>
@@ -1361,11 +1442,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>26</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1378,11 +1459,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>27</v>
       </c>
-      <c r="B30" s="31"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="4" t="s">
         <v>15</v>
       </c>
@@ -1393,11 +1474,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>28</v>
       </c>
-      <c r="B31" s="31"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="4" t="s">
         <v>4</v>
       </c>
@@ -1408,11 +1489,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>29</v>
       </c>
-      <c r="B32" s="31"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="4" t="s">
         <v>5</v>
       </c>
@@ -1423,25 +1504,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
-      <c r="B33" s="31"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="16"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="D34" s="17" t="s">
         <v>55</v>
       </c>
@@ -1449,11 +1530,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>30</v>
       </c>
-      <c r="B35" s="32"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="4" t="s">
         <v>6</v>
       </c>
@@ -1464,11 +1545,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>31</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -1477,66 +1558,66 @@
       <c r="D36" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E36" s="29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>32</v>
       </c>
-      <c r="B37" s="31"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="30"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>33</v>
       </c>
-      <c r="B38" s="31"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="26"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E38" s="30"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>34</v>
       </c>
-      <c r="B39" s="31"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="26"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E39" s="30"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>35</v>
       </c>
-      <c r="B40" s="32"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="27"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E40" s="31"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
-      <c r="B41" s="30" t="s">
-        <v>90</v>
+      <c r="B41" s="25" t="s">
+        <v>89</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>71</v>
@@ -1548,9 +1629,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
-      <c r="B42" s="31"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="4" t="s">
         <v>15</v>
       </c>
@@ -1561,9 +1642,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
-      <c r="B43" s="31"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="4" t="s">
         <v>4</v>
       </c>
@@ -1574,9 +1655,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
-      <c r="B44" s="31"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="4" t="s">
         <v>5</v>
       </c>
@@ -1587,9 +1668,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
-      <c r="B45" s="31"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="4" t="s">
         <v>6</v>
       </c>
@@ -1600,11 +1681,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>36</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="26" t="s">
         <v>14</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -1614,14 +1695,14 @@
         <v>81</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>37</v>
       </c>
-      <c r="B47" s="31"/>
+      <c r="B47" s="26"/>
       <c r="C47" s="4" t="s">
         <v>76</v>
       </c>
@@ -1632,11 +1713,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>38</v>
       </c>
-      <c r="B48" s="31"/>
+      <c r="B48" s="26"/>
       <c r="C48" s="4" t="s">
         <v>77</v>
       </c>
@@ -1647,11 +1728,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>39</v>
       </c>
-      <c r="B49" s="31"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="4" t="s">
         <v>78</v>
       </c>
@@ -1659,14 +1740,14 @@
         <v>55</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>40</v>
       </c>
-      <c r="B50" s="31"/>
+      <c r="B50" s="26"/>
       <c r="C50" s="4" t="s">
         <v>16</v>
       </c>
@@ -1677,11 +1758,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>41</v>
       </c>
-      <c r="B51" s="31"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="4" t="s">
         <v>18</v>
       </c>
@@ -1689,14 +1770,14 @@
         <v>55</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>42</v>
       </c>
-      <c r="B52" s="31"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="4" t="s">
         <v>19</v>
       </c>
@@ -1707,11 +1788,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>43</v>
       </c>
-      <c r="B53" s="31"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="4" t="s">
         <v>21</v>
       </c>
@@ -1722,11 +1803,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>44</v>
       </c>
-      <c r="B54" s="32"/>
+      <c r="B54" s="27"/>
       <c r="C54" s="4" t="s">
         <v>20</v>
       </c>
@@ -1737,11 +1818,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>45</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -1751,14 +1832,14 @@
         <v>55</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>46</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="4" t="s">
         <v>24</v>
       </c>
@@ -1766,14 +1847,14 @@
         <v>55</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
         <v>47</v>
       </c>
-      <c r="B57" s="29"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="4" t="s">
         <v>26</v>
       </c>
@@ -1781,14 +1862,14 @@
         <v>55</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>48</v>
       </c>
-      <c r="B58" s="29"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="4" t="s">
         <v>25</v>
       </c>
@@ -1796,14 +1877,14 @@
         <v>81</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>49</v>
       </c>
-      <c r="B59" s="29"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="4" t="s">
         <v>27</v>
       </c>
@@ -1811,14 +1892,14 @@
         <v>81</v>
       </c>
       <c r="E59" s="20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
         <v>50</v>
       </c>
-      <c r="B60" s="29"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="4" t="s">
         <v>19</v>
       </c>
@@ -1829,11 +1910,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>51</v>
       </c>
-      <c r="B61" s="29" t="s">
+      <c r="B61" s="28" t="s">
         <v>28</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -1846,11 +1927,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>52</v>
       </c>
-      <c r="B62" s="29"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="4" t="s">
         <v>18</v>
       </c>
@@ -1858,14 +1939,14 @@
         <v>81</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
         <v>53</v>
       </c>
-      <c r="B63" s="29"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="4" t="s">
         <v>16</v>
       </c>
@@ -1876,11 +1957,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>54</v>
       </c>
-      <c r="B64" s="29"/>
+      <c r="B64" s="28"/>
       <c r="C64" s="4" t="s">
         <v>19</v>
       </c>
@@ -1891,11 +1972,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>55</v>
       </c>
-      <c r="B65" s="29"/>
+      <c r="B65" s="28"/>
       <c r="C65" s="4" t="s">
         <v>29</v>
       </c>
@@ -1906,7 +1987,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="16">
         <v>56</v>
       </c>
@@ -1921,11 +2002,11 @@
       </c>
       <c r="E66" s="20"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <v>57</v>
       </c>
-      <c r="B67" s="29" t="s">
+      <c r="B67" s="28" t="s">
         <v>32</v>
       </c>
       <c r="C67" s="4" t="s">
@@ -1938,11 +2019,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>58</v>
       </c>
-      <c r="B68" s="29"/>
+      <c r="B68" s="28"/>
       <c r="C68" s="4" t="s">
         <v>16</v>
       </c>
@@ -1950,14 +2031,14 @@
         <v>81</v>
       </c>
       <c r="E68" s="20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
         <v>59</v>
       </c>
-      <c r="B69" s="29"/>
+      <c r="B69" s="28"/>
       <c r="C69" s="4" t="s">
         <v>19</v>
       </c>
@@ -1968,11 +2049,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <v>60</v>
       </c>
-      <c r="B70" s="29" t="s">
+      <c r="B70" s="28" t="s">
         <v>33</v>
       </c>
       <c r="C70" s="4" t="s">
@@ -1982,14 +2063,14 @@
         <v>81</v>
       </c>
       <c r="E70" s="20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>61</v>
       </c>
-      <c r="B71" s="29"/>
+      <c r="B71" s="28"/>
       <c r="C71" s="4" t="s">
         <v>16</v>
       </c>
@@ -1997,14 +2078,14 @@
         <v>81</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="16">
         <v>62</v>
       </c>
-      <c r="B72" s="29"/>
+      <c r="B72" s="28"/>
       <c r="C72" s="4" t="s">
         <v>19</v>
       </c>
@@ -2012,10 +2093,10 @@
         <v>81</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>63</v>
       </c>
@@ -2032,11 +2113,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <v>64</v>
       </c>
-      <c r="B74" s="29" t="s">
+      <c r="B74" s="28" t="s">
         <v>36</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -2049,11 +2130,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="16">
         <v>65</v>
       </c>
-      <c r="B75" s="29"/>
+      <c r="B75" s="28"/>
       <c r="C75" s="4" t="s">
         <v>16</v>
       </c>
@@ -2064,11 +2145,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <v>66</v>
       </c>
-      <c r="B76" s="29"/>
+      <c r="B76" s="28"/>
       <c r="C76" s="4" t="s">
         <v>19</v>
       </c>
@@ -2079,11 +2160,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>67</v>
       </c>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -2093,14 +2174,14 @@
         <v>81</v>
       </c>
       <c r="E77" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
         <v>68</v>
       </c>
-      <c r="B78" s="32"/>
+      <c r="B78" s="27"/>
       <c r="C78" s="4" t="s">
         <v>43</v>
       </c>
@@ -2111,11 +2192,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <v>69</v>
       </c>
-      <c r="B79" s="30" t="s">
+      <c r="B79" s="25" t="s">
         <v>38</v>
       </c>
       <c r="C79" s="4" t="s">
@@ -2125,14 +2206,14 @@
         <v>81</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <v>70</v>
       </c>
-      <c r="B80" s="32"/>
+      <c r="B80" s="27"/>
       <c r="C80" s="4" t="s">
         <v>43</v>
       </c>
@@ -2140,15 +2221,15 @@
         <v>81</v>
       </c>
       <c r="E80" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16">
         <v>71</v>
       </c>
-      <c r="B81" s="30" t="s">
-        <v>110</v>
+      <c r="B81" s="25" t="s">
+        <v>108</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>42</v>
@@ -2160,11 +2241,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <v>72</v>
       </c>
-      <c r="B82" s="32"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="4" t="s">
         <v>43</v>
       </c>
@@ -2175,11 +2256,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <v>73</v>
       </c>
-      <c r="B83" s="30" t="s">
+      <c r="B83" s="25" t="s">
         <v>39</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -2192,11 +2273,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
         <v>74</v>
       </c>
-      <c r="B84" s="32"/>
+      <c r="B84" s="27"/>
       <c r="C84" s="4" t="s">
         <v>43</v>
       </c>
@@ -2205,11 +2286,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <v>75</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B85" s="25" t="s">
         <v>40</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -2219,14 +2300,14 @@
         <v>81</v>
       </c>
       <c r="E85" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <v>76</v>
       </c>
-      <c r="B86" s="31"/>
+      <c r="B86" s="26"/>
       <c r="C86" s="4" t="s">
         <v>43</v>
       </c>
@@ -2237,11 +2318,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="16">
         <v>77</v>
       </c>
-      <c r="B87" s="32"/>
+      <c r="B87" s="27"/>
       <c r="C87" s="4" t="s">
         <v>45</v>
       </c>
@@ -2252,11 +2333,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <v>78</v>
       </c>
-      <c r="B88" s="30" t="s">
+      <c r="B88" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C88" s="4" t="s">
@@ -2266,14 +2347,14 @@
         <v>81</v>
       </c>
       <c r="E88" s="20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <v>79</v>
       </c>
-      <c r="B89" s="32"/>
+      <c r="B89" s="27"/>
       <c r="C89" s="4" t="s">
         <v>43</v>
       </c>
@@ -2284,11 +2365,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
         <v>80</v>
       </c>
-      <c r="B90" s="30" t="s">
+      <c r="B90" s="25" t="s">
         <v>47</v>
       </c>
       <c r="C90" s="4" t="s">
@@ -2298,14 +2379,14 @@
         <v>81</v>
       </c>
       <c r="E90" s="20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <v>81</v>
       </c>
-      <c r="B91" s="32"/>
+      <c r="B91" s="27"/>
       <c r="C91" s="4" t="s">
         <v>45</v>
       </c>
@@ -2313,14 +2394,14 @@
         <v>81</v>
       </c>
       <c r="E91" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <v>82</v>
       </c>
-      <c r="B92" s="30" t="s">
+      <c r="B92" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C92" s="4" t="s">
@@ -2330,14 +2411,14 @@
         <v>81</v>
       </c>
       <c r="E92" s="20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="16">
         <v>83</v>
       </c>
-      <c r="B93" s="32"/>
+      <c r="B93" s="27"/>
       <c r="C93" s="4" t="s">
         <v>45</v>
       </c>
@@ -2345,14 +2426,14 @@
         <v>81</v>
       </c>
       <c r="E93" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <v>84</v>
       </c>
-      <c r="B94" s="30" t="s">
+      <c r="B94" s="25" t="s">
         <v>51</v>
       </c>
       <c r="C94" s="4" t="s">
@@ -2362,14 +2443,14 @@
         <v>81</v>
       </c>
       <c r="E94" s="20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <v>85</v>
       </c>
-      <c r="B95" s="32"/>
+      <c r="B95" s="27"/>
       <c r="C95" s="4" t="s">
         <v>45</v>
       </c>
@@ -2377,14 +2458,14 @@
         <v>81</v>
       </c>
       <c r="E95" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="16">
         <v>86</v>
       </c>
-      <c r="B96" s="30" t="s">
+      <c r="B96" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C96" s="4" t="s">
@@ -2397,11 +2478,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <v>87</v>
       </c>
-      <c r="B97" s="32"/>
+      <c r="B97" s="27"/>
       <c r="C97" s="4" t="s">
         <v>43</v>
       </c>
@@ -2412,7 +2493,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <v>88</v>
       </c>
@@ -2429,7 +2510,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="16">
         <v>89</v>
       </c>
@@ -2444,7 +2525,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <v>90</v>
       </c>
@@ -2456,10 +2537,10 @@
         <v>81</v>
       </c>
       <c r="E100" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <v>91</v>
       </c>
@@ -2471,10 +2552,10 @@
         <v>55</v>
       </c>
       <c r="E101" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="16">
         <v>92</v>
       </c>
@@ -2486,10 +2567,10 @@
         <v>55</v>
       </c>
       <c r="E102" s="21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <v>93</v>
       </c>
@@ -2504,7 +2585,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <v>94</v>
       </c>
@@ -2516,29 +2597,12 @@
         <v>81</v>
       </c>
       <c r="E104" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:E103" xr:uid="{C0E55FD2-3E6D-4E64-946D-647C70AEE35D}"/>
   <mergeCells count="29">
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="B46:B54"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B85:B87"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B55:B60"/>
     <mergeCell ref="E36:E40"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
@@ -2551,6 +2615,23 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="B36:B40"/>
     <mergeCell ref="B29:B35"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B46:B54"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B55:B60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2565,14 +2646,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.36328125" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>82</v>
       </c>
@@ -2581,20 +2662,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>